<commit_message>
Final Update For V2
</commit_message>
<xml_diff>
--- a/app/accounting/402000AD/PCE INV 402031.xlsx
+++ b/app/accounting/402000AD/PCE INV 402031.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\00-Bridge Database\402000AD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\xero-asana-integration\app\accounting\402000AD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC345225-07FD-46E6-B76A-197C30929B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84CC781-936C-44D8-9F50-8D108FDE4963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18240" yWindow="5520" windowWidth="16200" windowHeight="7200" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
+    <workbookView xWindow="32760" yWindow="135" windowWidth="21600" windowHeight="11505" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="13" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Date:</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t xml:space="preserve">Total: </t>
+  </si>
+  <si>
+    <t>Variation</t>
+  </si>
+  <si>
+    <t>V1</t>
   </si>
 </sst>
 </file>
@@ -644,9 +650,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +690,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -790,7 +796,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -932,7 +938,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -999,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="45">
-        <v>45337</v>
+        <v>45362</v>
       </c>
       <c r="K4" s="43"/>
       <c r="L4" s="7"/>
@@ -1261,7 +1267,9 @@
       <c r="S19" s="34"/>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+      <c r="A20" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
       <c r="H20" s="48"/>
@@ -1271,9 +1279,13 @@
       <c r="S20" s="37"/>
     </row>
     <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
+      <c r="A21" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="G21" s="53">
+        <v>100</v>
+      </c>
       <c r="H21" s="48"/>
       <c r="I21" s="23"/>
       <c r="J21" s="23"/>

</xml_diff>